<commit_message>
Updated pinout spreadsheet and added Ethernet Phy device to library.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/Document/Connector Bus Signals.xlsx
+++ b/hardware/MainBoard/Document/Connector Bus Signals.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="59">
   <si>
     <t>Pin</t>
   </si>
@@ -47695,10 +47695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48297,7 +48297,7 @@
       </c>
       <c r="J17" s="4"/>
       <c r="M17" s="4" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="N17" s="4">
         <v>29</v>
@@ -48306,7 +48306,7 @@
         <v>30</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -48331,7 +48331,7 @@
       </c>
       <c r="J18" s="4"/>
       <c r="M18" s="4" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="N18" s="4">
         <v>31</v>
@@ -48340,7 +48340,7 @@
         <v>32</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -48399,7 +48399,7 @@
       </c>
       <c r="J20" s="4"/>
       <c r="M20" s="4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="N20" s="4">
         <v>35</v>
@@ -48408,7 +48408,7 @@
         <v>36</v>
       </c>
       <c r="P20" s="4" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -48435,7 +48435,7 @@
       </c>
       <c r="J21" s="4"/>
       <c r="M21" s="4" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="N21" s="4">
         <v>37</v>
@@ -48444,7 +48444,7 @@
         <v>38</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -48507,7 +48507,7 @@
       </c>
       <c r="J23" s="4"/>
       <c r="M23" s="4" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="N23" s="4">
         <v>41</v>
@@ -48516,7 +48516,7 @@
         <v>42</v>
       </c>
       <c r="P23" s="4" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
@@ -48545,7 +48545,7 @@
         <v>5</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="N24" s="4">
         <v>43</v>
@@ -48554,7 +48554,7 @@
         <v>44</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
@@ -48621,7 +48621,7 @@
         <v>44</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="N26" s="4">
         <v>47</v>
@@ -48630,7 +48630,7 @@
         <v>48</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
@@ -48659,7 +48659,7 @@
         <v>5</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="N27" s="4">
         <v>49</v>
@@ -48668,7 +48668,7 @@
         <v>50</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
@@ -48735,7 +48735,7 @@
         <v>43</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="N29" s="4">
         <v>53</v>
@@ -48744,7 +48744,7 @@
         <v>54</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
@@ -48773,7 +48773,7 @@
         <v>5</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="N30" s="4">
         <v>55</v>
@@ -48782,7 +48782,7 @@
         <v>56</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
@@ -48845,7 +48845,7 @@
         <v>53</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="N32" s="4">
         <v>59</v>
@@ -48854,7 +48854,7 @@
         <v>60</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
@@ -48883,7 +48883,7 @@
         <v>5</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="N33" s="4">
         <v>61</v>
@@ -48892,7 +48892,7 @@
         <v>62</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
@@ -48947,7 +48947,7 @@
         <v>52</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="N35" s="4">
         <v>65</v>
@@ -48956,7 +48956,7 @@
         <v>66</v>
       </c>
       <c r="P35" s="4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
@@ -48973,7 +48973,7 @@
         <v>5</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="N36" s="4">
         <v>67</v>
@@ -48982,7 +48982,7 @@
         <v>68</v>
       </c>
       <c r="P36" s="4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
@@ -49025,7 +49025,7 @@
         <v>5</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="N38" s="4">
         <v>71</v>
@@ -49034,7 +49034,7 @@
         <v>72</v>
       </c>
       <c r="P38" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
@@ -49051,7 +49051,7 @@
         <v>5</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="N39" s="4">
         <v>73</v>
@@ -49060,7 +49060,7 @@
         <v>74</v>
       </c>
       <c r="P39" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
@@ -49189,146 +49189,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H45" s="4">
-        <v>85</v>
-      </c>
-      <c r="I45" s="4">
-        <v>86</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G46" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H46" s="4">
-        <v>87</v>
-      </c>
-      <c r="I46" s="4">
-        <v>88</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G47" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H47" s="4">
-        <v>89</v>
-      </c>
-      <c r="I47" s="4">
-        <v>90</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G48" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H48" s="4">
-        <v>91</v>
-      </c>
-      <c r="I48" s="4">
-        <v>92</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-    </row>
-    <row r="49" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G49" s="4"/>
-      <c r="H49" s="4">
-        <v>93</v>
-      </c>
-      <c r="I49" s="4">
-        <v>94</v>
-      </c>
-      <c r="J49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-    </row>
-    <row r="50" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="4">
-        <v>95</v>
-      </c>
-      <c r="I50" s="4">
-        <v>96</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-      <c r="P50" s="4"/>
-    </row>
-    <row r="51" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G51" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H51" s="4">
-        <v>97</v>
-      </c>
-      <c r="I51" s="4">
-        <v>98</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-      <c r="P51" s="4"/>
-    </row>
-    <row r="52" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G52" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H52" s="4">
-        <v>99</v>
-      </c>
-      <c r="I52" s="4">
-        <v>100</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M52" s="4"/>
-      <c r="N52" s="4"/>
-      <c r="O52" s="4"/>
-      <c r="P52" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B1:E1"/>
@@ -49583,7 +49443,7 @@
       <formula>LEN(TRIM(E12))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J10 J40 G46:G47 G1:G13 J34:J35 H1:I52">
+  <conditionalFormatting sqref="J1:J10 J40 G1:G13 J34:J35 H1:I44">
     <cfRule type="containsText" dxfId="4664" priority="5641" operator="containsText" text="GPIO">
       <formula>NOT(ISERROR(SEARCH("GPIO",G1)))</formula>
     </cfRule>
@@ -49627,7 +49487,7 @@
       <formula>NOT(ISERROR(SEARCH("AGND",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J10 G46:G47 J40 G3:G13 J34:J35">
+  <conditionalFormatting sqref="J3:J10 J40 G3:G13 J34:J35">
     <cfRule type="containsBlanks" dxfId="4650" priority="5655">
       <formula>LEN(TRIM(G3))=0</formula>
     </cfRule>
@@ -49779,153 +49639,6 @@
       <formula>LEN(TRIM(J12))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G48:G52 J48:J52">
-    <cfRule type="containsText" dxfId="4604" priority="5566" operator="containsText" text="GPIO">
-      <formula>NOT(ISERROR(SEARCH("GPIO",G48)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4603" priority="5567" operator="beginsWith" text="PC">
-      <formula>LEFT(G48,2)="PC"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4602" priority="5568" operator="beginsWith" text="PB">
-      <formula>LEFT(G48,2)="PB"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4601" priority="5569" operator="beginsWith" text="PA">
-      <formula>LEFT(G48,2)="PA"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4600" priority="5570" operator="containsText" text="I2C">
-      <formula>NOT(ISERROR(SEARCH("I2C",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4599" priority="5571" operator="containsText" text="SPI">
-      <formula>NOT(ISERROR(SEARCH("SPI",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4598" priority="5572" operator="containsText" text="DXVY">
-      <formula>NOT(ISERROR(SEARCH("DXVY",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4597" priority="5573" operator="containsText" text="D1V5">
-      <formula>NOT(ISERROR(SEARCH("D1V5",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4596" priority="5574" operator="containsText" text="D3V3">
-      <formula>NOT(ISERROR(SEARCH("D3V3",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4595" priority="5575" operator="containsText" text="VSUP">
-      <formula>NOT(ISERROR(SEARCH("VSUP",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4594" priority="5576" operator="containsText" text="DGND">
-      <formula>NOT(ISERROR(SEARCH("DGND",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4593" priority="5577" operator="containsText" text="A1V5">
-      <formula>NOT(ISERROR(SEARCH("A1V5",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4592" priority="5578" operator="containsText" text="A3V3">
-      <formula>NOT(ISERROR(SEARCH("A3V3",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4591" priority="5579" operator="containsText" text="AGND">
-      <formula>NOT(ISERROR(SEARCH("AGND",G48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J48:J52 G48:G52">
-    <cfRule type="containsBlanks" dxfId="4590" priority="5580">
-      <formula>LEN(TRIM(G48))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J45">
-    <cfRule type="containsText" dxfId="4589" priority="5521" operator="containsText" text="GPIO">
-      <formula>NOT(ISERROR(SEARCH("GPIO",J45)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4588" priority="5522" operator="beginsWith" text="PC">
-      <formula>LEFT(J45,2)="PC"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4587" priority="5523" operator="beginsWith" text="PB">
-      <formula>LEFT(J45,2)="PB"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4586" priority="5524" operator="beginsWith" text="PA">
-      <formula>LEFT(J45,2)="PA"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4585" priority="5525" operator="containsText" text="I2C">
-      <formula>NOT(ISERROR(SEARCH("I2C",J45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4584" priority="5526" operator="containsText" text="SPI">
-      <formula>NOT(ISERROR(SEARCH("SPI",J45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4583" priority="5527" operator="containsText" text="DXVY">
-      <formula>NOT(ISERROR(SEARCH("DXVY",J45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4582" priority="5528" operator="containsText" text="D1V5">
-      <formula>NOT(ISERROR(SEARCH("D1V5",J45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4581" priority="5529" operator="containsText" text="D3V3">
-      <formula>NOT(ISERROR(SEARCH("D3V3",J45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4580" priority="5530" operator="containsText" text="VSUP">
-      <formula>NOT(ISERROR(SEARCH("VSUP",J45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4579" priority="5531" operator="containsText" text="DGND">
-      <formula>NOT(ISERROR(SEARCH("DGND",J45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4578" priority="5532" operator="containsText" text="A1V5">
-      <formula>NOT(ISERROR(SEARCH("A1V5",J45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4577" priority="5533" operator="containsText" text="A3V3">
-      <formula>NOT(ISERROR(SEARCH("A3V3",J45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4576" priority="5534" operator="containsText" text="AGND">
-      <formula>NOT(ISERROR(SEARCH("AGND",J45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J45">
-    <cfRule type="containsBlanks" dxfId="4575" priority="5535">
-      <formula>LEN(TRIM(J45))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="4574" priority="5506" operator="containsText" text="GPIO">
-      <formula>NOT(ISERROR(SEARCH("GPIO",G45)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4573" priority="5507" operator="beginsWith" text="PC">
-      <formula>LEFT(G45,2)="PC"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4572" priority="5508" operator="beginsWith" text="PB">
-      <formula>LEFT(G45,2)="PB"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4571" priority="5509" operator="beginsWith" text="PA">
-      <formula>LEFT(G45,2)="PA"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4570" priority="5510" operator="containsText" text="I2C">
-      <formula>NOT(ISERROR(SEARCH("I2C",G45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4569" priority="5511" operator="containsText" text="SPI">
-      <formula>NOT(ISERROR(SEARCH("SPI",G45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4568" priority="5512" operator="containsText" text="DXVY">
-      <formula>NOT(ISERROR(SEARCH("DXVY",G45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4567" priority="5513" operator="containsText" text="D1V5">
-      <formula>NOT(ISERROR(SEARCH("D1V5",G45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4566" priority="5514" operator="containsText" text="D3V3">
-      <formula>NOT(ISERROR(SEARCH("D3V3",G45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4565" priority="5515" operator="containsText" text="VSUP">
-      <formula>NOT(ISERROR(SEARCH("VSUP",G45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4564" priority="5516" operator="containsText" text="DGND">
-      <formula>NOT(ISERROR(SEARCH("DGND",G45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4563" priority="5517" operator="containsText" text="A1V5">
-      <formula>NOT(ISERROR(SEARCH("A1V5",G45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4562" priority="5518" operator="containsText" text="A3V3">
-      <formula>NOT(ISERROR(SEARCH("A3V3",G45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4561" priority="5519" operator="containsText" text="AGND">
-      <formula>NOT(ISERROR(SEARCH("AGND",G45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
-    <cfRule type="containsBlanks" dxfId="4560" priority="5520">
-      <formula>LEN(TRIM(G45))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G42:G44">
     <cfRule type="containsText" dxfId="4559" priority="5491" operator="containsText" text="GPIO">
       <formula>NOT(ISERROR(SEARCH("GPIO",G42)))</formula>
@@ -52425,55 +52138,6 @@
       <formula>LEN(TRIM(J14))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J46:J47">
-    <cfRule type="containsText" dxfId="3794" priority="4291" operator="containsText" text="GPIO">
-      <formula>NOT(ISERROR(SEARCH("GPIO",J46)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3793" priority="4292" operator="beginsWith" text="PC">
-      <formula>LEFT(J46,2)="PC"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3792" priority="4293" operator="beginsWith" text="PB">
-      <formula>LEFT(J46,2)="PB"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3791" priority="4294" operator="beginsWith" text="PA">
-      <formula>LEFT(J46,2)="PA"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3790" priority="4295" operator="containsText" text="I2C">
-      <formula>NOT(ISERROR(SEARCH("I2C",J46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3789" priority="4296" operator="containsText" text="SPI">
-      <formula>NOT(ISERROR(SEARCH("SPI",J46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3788" priority="4297" operator="containsText" text="DXVY">
-      <formula>NOT(ISERROR(SEARCH("DXVY",J46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3787" priority="4298" operator="containsText" text="D1V5">
-      <formula>NOT(ISERROR(SEARCH("D1V5",J46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3786" priority="4299" operator="containsText" text="D3V3">
-      <formula>NOT(ISERROR(SEARCH("D3V3",J46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3785" priority="4300" operator="containsText" text="VSUP">
-      <formula>NOT(ISERROR(SEARCH("VSUP",J46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3784" priority="4301" operator="containsText" text="DGND">
-      <formula>NOT(ISERROR(SEARCH("DGND",J46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3783" priority="4302" operator="containsText" text="A1V5">
-      <formula>NOT(ISERROR(SEARCH("A1V5",J46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3782" priority="4303" operator="containsText" text="A3V3">
-      <formula>NOT(ISERROR(SEARCH("A3V3",J46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3781" priority="4304" operator="containsText" text="AGND">
-      <formula>NOT(ISERROR(SEARCH("AGND",J46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J46:J47">
-    <cfRule type="containsBlanks" dxfId="3780" priority="4305">
-      <formula>LEN(TRIM(J46))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J43:J44">
     <cfRule type="containsText" dxfId="3779" priority="4216" operator="containsText" text="GPIO">
       <formula>NOT(ISERROR(SEARCH("GPIO",J43)))</formula>
@@ -55267,7 +54931,7 @@
       <formula>LEN(TRIM(G23))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P10 P40 M46:M47 P34:P35 N1:O52 M1:M13">
+  <conditionalFormatting sqref="P1:P10 P40 P34:P35 N1:O44 M1:M13">
     <cfRule type="containsText" dxfId="2924" priority="2986" operator="containsText" text="GPIO">
       <formula>NOT(ISERROR(SEARCH("GPIO",M1)))</formula>
     </cfRule>
@@ -55311,7 +54975,7 @@
       <formula>NOT(ISERROR(SEARCH("AGND",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P10 M46:M47 P40 P34:P35 M3:M13">
+  <conditionalFormatting sqref="P3:P10 P40 P34:P35 M3:M13">
     <cfRule type="containsBlanks" dxfId="2910" priority="3000">
       <formula>LEN(TRIM(M3))=0</formula>
     </cfRule>
@@ -55414,153 +55078,6 @@
       <formula>LEN(TRIM(P12))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M48:M52 P48:P52">
-    <cfRule type="containsText" dxfId="2879" priority="2926" operator="containsText" text="GPIO">
-      <formula>NOT(ISERROR(SEARCH("GPIO",M48)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2878" priority="2927" operator="beginsWith" text="PC">
-      <formula>LEFT(M48,2)="PC"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2877" priority="2928" operator="beginsWith" text="PB">
-      <formula>LEFT(M48,2)="PB"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2876" priority="2929" operator="beginsWith" text="PA">
-      <formula>LEFT(M48,2)="PA"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2875" priority="2930" operator="containsText" text="I2C">
-      <formula>NOT(ISERROR(SEARCH("I2C",M48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2874" priority="2931" operator="containsText" text="SPI">
-      <formula>NOT(ISERROR(SEARCH("SPI",M48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2873" priority="2932" operator="containsText" text="DXVY">
-      <formula>NOT(ISERROR(SEARCH("DXVY",M48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2872" priority="2933" operator="containsText" text="D1V5">
-      <formula>NOT(ISERROR(SEARCH("D1V5",M48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2871" priority="2934" operator="containsText" text="D3V3">
-      <formula>NOT(ISERROR(SEARCH("D3V3",M48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2870" priority="2935" operator="containsText" text="VSUP">
-      <formula>NOT(ISERROR(SEARCH("VSUP",M48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2869" priority="2936" operator="containsText" text="DGND">
-      <formula>NOT(ISERROR(SEARCH("DGND",M48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2868" priority="2937" operator="containsText" text="A1V5">
-      <formula>NOT(ISERROR(SEARCH("A1V5",M48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2867" priority="2938" operator="containsText" text="A3V3">
-      <formula>NOT(ISERROR(SEARCH("A3V3",M48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2866" priority="2939" operator="containsText" text="AGND">
-      <formula>NOT(ISERROR(SEARCH("AGND",M48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P48:P52 M48:M52">
-    <cfRule type="containsBlanks" dxfId="2865" priority="2940">
-      <formula>LEN(TRIM(M48))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P45">
-    <cfRule type="containsText" dxfId="2864" priority="2911" operator="containsText" text="GPIO">
-      <formula>NOT(ISERROR(SEARCH("GPIO",P45)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2863" priority="2912" operator="beginsWith" text="PC">
-      <formula>LEFT(P45,2)="PC"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2862" priority="2913" operator="beginsWith" text="PB">
-      <formula>LEFT(P45,2)="PB"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2861" priority="2914" operator="beginsWith" text="PA">
-      <formula>LEFT(P45,2)="PA"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2860" priority="2915" operator="containsText" text="I2C">
-      <formula>NOT(ISERROR(SEARCH("I2C",P45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2859" priority="2916" operator="containsText" text="SPI">
-      <formula>NOT(ISERROR(SEARCH("SPI",P45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2858" priority="2917" operator="containsText" text="DXVY">
-      <formula>NOT(ISERROR(SEARCH("DXVY",P45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2857" priority="2918" operator="containsText" text="D1V5">
-      <formula>NOT(ISERROR(SEARCH("D1V5",P45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2856" priority="2919" operator="containsText" text="D3V3">
-      <formula>NOT(ISERROR(SEARCH("D3V3",P45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2855" priority="2920" operator="containsText" text="VSUP">
-      <formula>NOT(ISERROR(SEARCH("VSUP",P45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2854" priority="2921" operator="containsText" text="DGND">
-      <formula>NOT(ISERROR(SEARCH("DGND",P45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2853" priority="2922" operator="containsText" text="A1V5">
-      <formula>NOT(ISERROR(SEARCH("A1V5",P45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2852" priority="2923" operator="containsText" text="A3V3">
-      <formula>NOT(ISERROR(SEARCH("A3V3",P45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2851" priority="2924" operator="containsText" text="AGND">
-      <formula>NOT(ISERROR(SEARCH("AGND",P45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P45">
-    <cfRule type="containsBlanks" dxfId="2850" priority="2925">
-      <formula>LEN(TRIM(P45))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M45">
-    <cfRule type="containsText" dxfId="2849" priority="2896" operator="containsText" text="GPIO">
-      <formula>NOT(ISERROR(SEARCH("GPIO",M45)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2848" priority="2897" operator="beginsWith" text="PC">
-      <formula>LEFT(M45,2)="PC"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2847" priority="2898" operator="beginsWith" text="PB">
-      <formula>LEFT(M45,2)="PB"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2846" priority="2899" operator="beginsWith" text="PA">
-      <formula>LEFT(M45,2)="PA"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2845" priority="2900" operator="containsText" text="I2C">
-      <formula>NOT(ISERROR(SEARCH("I2C",M45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2844" priority="2901" operator="containsText" text="SPI">
-      <formula>NOT(ISERROR(SEARCH("SPI",M45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2843" priority="2902" operator="containsText" text="DXVY">
-      <formula>NOT(ISERROR(SEARCH("DXVY",M45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2842" priority="2903" operator="containsText" text="D1V5">
-      <formula>NOT(ISERROR(SEARCH("D1V5",M45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2841" priority="2904" operator="containsText" text="D3V3">
-      <formula>NOT(ISERROR(SEARCH("D3V3",M45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2840" priority="2905" operator="containsText" text="VSUP">
-      <formula>NOT(ISERROR(SEARCH("VSUP",M45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2839" priority="2906" operator="containsText" text="DGND">
-      <formula>NOT(ISERROR(SEARCH("DGND",M45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2838" priority="2907" operator="containsText" text="A1V5">
-      <formula>NOT(ISERROR(SEARCH("A1V5",M45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2837" priority="2908" operator="containsText" text="A3V3">
-      <formula>NOT(ISERROR(SEARCH("A3V3",M45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2836" priority="2909" operator="containsText" text="AGND">
-      <formula>NOT(ISERROR(SEARCH("AGND",M45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M45">
-    <cfRule type="containsBlanks" dxfId="2835" priority="2910">
-      <formula>LEN(TRIM(M45))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M42:M44">
     <cfRule type="containsText" dxfId="2834" priority="2881" operator="containsText" text="GPIO">
       <formula>NOT(ISERROR(SEARCH("GPIO",M42)))</formula>
@@ -57960,55 +57477,6 @@
   <conditionalFormatting sqref="M14">
     <cfRule type="containsBlanks" dxfId="2100" priority="2175">
       <formula>LEN(TRIM(M14))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P46:P47">
-    <cfRule type="containsText" dxfId="2099" priority="2116" operator="containsText" text="GPIO">
-      <formula>NOT(ISERROR(SEARCH("GPIO",P46)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2098" priority="2117" operator="beginsWith" text="PC">
-      <formula>LEFT(P46,2)="PC"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2097" priority="2118" operator="beginsWith" text="PB">
-      <formula>LEFT(P46,2)="PB"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2096" priority="2119" operator="beginsWith" text="PA">
-      <formula>LEFT(P46,2)="PA"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2095" priority="2120" operator="containsText" text="I2C">
-      <formula>NOT(ISERROR(SEARCH("I2C",P46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2094" priority="2121" operator="containsText" text="SPI">
-      <formula>NOT(ISERROR(SEARCH("SPI",P46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2093" priority="2122" operator="containsText" text="DXVY">
-      <formula>NOT(ISERROR(SEARCH("DXVY",P46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2092" priority="2123" operator="containsText" text="D1V5">
-      <formula>NOT(ISERROR(SEARCH("D1V5",P46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2091" priority="2124" operator="containsText" text="D3V3">
-      <formula>NOT(ISERROR(SEARCH("D3V3",P46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2090" priority="2125" operator="containsText" text="VSUP">
-      <formula>NOT(ISERROR(SEARCH("VSUP",P46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2089" priority="2126" operator="containsText" text="DGND">
-      <formula>NOT(ISERROR(SEARCH("DGND",P46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2088" priority="2127" operator="containsText" text="A1V5">
-      <formula>NOT(ISERROR(SEARCH("A1V5",P46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2087" priority="2128" operator="containsText" text="A3V3">
-      <formula>NOT(ISERROR(SEARCH("A3V3",P46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2086" priority="2129" operator="containsText" text="AGND">
-      <formula>NOT(ISERROR(SEARCH("AGND",P46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P46:P47">
-    <cfRule type="containsBlanks" dxfId="2085" priority="2130">
-      <formula>LEN(TRIM(P46))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P43:P44">

</xml_diff>

<commit_message>
Routed MSS and FPGA I/O (GPIO) signals from the Mezzanine connector to SmartFusion.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/Document/Connector Bus Signals.xlsx
+++ b/hardware/MainBoard/Document/Connector Bus Signals.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="83">
   <si>
     <t>Pin</t>
   </si>
@@ -260,6 +260,12 @@
   <si>
     <t>NGPIO4</t>
   </si>
+  <si>
+    <t>SGPIO2</t>
+  </si>
+  <si>
+    <t>SGPIO5</t>
+  </si>
 </sst>
 </file>
 
@@ -436,7 +442,574 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8594">
+  <dxfs count="8675">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -85941,7 +86514,7 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -86143,7 +86716,9 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
+      <c r="C9" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="D9" s="3">
         <v>11</v>
       </c>
@@ -86170,7 +86745,9 @@
       </c>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
+      <c r="C10" s="12" t="s">
+        <v>74</v>
+      </c>
       <c r="D10" s="3">
         <v>13</v>
       </c>
@@ -86233,7 +86810,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C12" s="12" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D12" s="3">
         <v>17</v>
@@ -86265,7 +86842,7 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D13" s="3">
         <v>19</v>
@@ -86290,8 +86867,8 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C14" s="17" t="s">
-        <v>44</v>
+      <c r="C14" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="D14" s="3">
         <v>21</v>
@@ -86302,8 +86879,8 @@
       <c r="F14" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="J14" s="17" t="s">
-        <v>44</v>
+      <c r="J14" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="K14" s="3">
         <v>21</v>
@@ -86325,8 +86902,8 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="18" t="s">
-        <v>53</v>
+      <c r="C15" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="D15" s="3">
         <v>23</v>
@@ -86337,8 +86914,8 @@
       <c r="F15" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="J15" s="18" t="s">
-        <v>53</v>
+      <c r="J15" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="K15" s="3">
         <v>23</v>
@@ -86357,8 +86934,8 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C16" s="18" t="s">
-        <v>52</v>
+      <c r="C16" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="D16" s="3">
         <v>25</v>
@@ -86366,11 +86943,11 @@
       <c r="E16" s="3">
         <v>26</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>75</v>
+      <c r="F16" s="18" t="s">
+        <v>53</v>
       </c>
-      <c r="J16" s="18" t="s">
-        <v>52</v>
+      <c r="J16" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="K16" s="3">
         <v>25</v>
@@ -86378,8 +86955,8 @@
       <c r="L16" s="3">
         <v>26</v>
       </c>
-      <c r="M16" s="14" t="s">
-        <v>46</v>
+      <c r="M16" s="18" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="3:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -86392,8 +86969,8 @@
       <c r="E17" s="3">
         <v>28</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>76</v>
+      <c r="F17" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="J17" s="16" t="s">
         <v>45</v>
@@ -86404,8 +86981,8 @@
       <c r="L17" s="3">
         <v>28</v>
       </c>
-      <c r="M17" s="14" t="s">
-        <v>47</v>
+      <c r="M17" s="18" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -87053,33 +87630,62 @@
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="K3:L3"/>
   </mergeCells>
-  <conditionalFormatting sqref="J1:J1048576 M1:M1048576 F1:F1048576 C1:C8 C11:C1048576">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="DAC">
+  <conditionalFormatting sqref="C1:C8 F1:F1048576 C11:C1048576 M1:M1048576 J1:J1048576">
+    <cfRule type="containsText" dxfId="89" priority="10" operator="containsText" text="DAC">
       <formula>NOT(ISERROR(SEARCH("DAC",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="ADC">
+    <cfRule type="containsText" dxfId="88" priority="11" operator="containsText" text="ADC">
       <formula>NOT(ISERROR(SEARCH("ADC",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="D1V5">
+    <cfRule type="containsText" dxfId="87" priority="12" operator="containsText" text="D1V5">
       <formula>NOT(ISERROR(SEARCH("D1V5",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="D3V3">
+    <cfRule type="containsText" dxfId="86" priority="13" operator="containsText" text="D3V3">
       <formula>NOT(ISERROR(SEARCH("D3V3",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="VSUP">
+    <cfRule type="containsText" dxfId="85" priority="14" operator="containsText" text="VSUP">
       <formula>NOT(ISERROR(SEARCH("VSUP",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="DGND">
+    <cfRule type="containsText" dxfId="84" priority="15" operator="containsText" text="DGND">
       <formula>NOT(ISERROR(SEARCH("DGND",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="A3V3">
+    <cfRule type="containsText" dxfId="83" priority="16" operator="containsText" text="A3V3">
       <formula>NOT(ISERROR(SEARCH("A3V3",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="A1V5">
+    <cfRule type="containsText" dxfId="82" priority="17" operator="containsText" text="A1V5">
       <formula>NOT(ISERROR(SEARCH("A1V5",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="9" operator="containsText" text="AGND">
+    <cfRule type="containsText" dxfId="81" priority="18" operator="containsText" text="AGND">
       <formula>NOT(ISERROR(SEARCH("AGND",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:C10">
+    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="DAC">
+      <formula>NOT(ISERROR(SEARCH("DAC",C9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="ADC">
+      <formula>NOT(ISERROR(SEARCH("ADC",C9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="D1V5">
+      <formula>NOT(ISERROR(SEARCH("D1V5",C9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="D3V3">
+      <formula>NOT(ISERROR(SEARCH("D3V3",C9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="VSUP">
+      <formula>NOT(ISERROR(SEARCH("VSUP",C9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="DGND">
+      <formula>NOT(ISERROR(SEARCH("DGND",C9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="7" operator="containsText" text="A3V3">
+      <formula>NOT(ISERROR(SEARCH("A3V3",C9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="8" operator="containsText" text="A1V5">
+      <formula>NOT(ISERROR(SEARCH("A1V5",C9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="9" operator="containsText" text="AGND">
+      <formula>NOT(ISERROR(SEARCH("AGND",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>